<commit_message>
more studies, nearly finished
</commit_message>
<xml_diff>
--- a/data/meta_table_filled_280319.xlsx
+++ b/data/meta_table_filled_280319.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="31520" yWindow="3300" windowWidth="32920" windowHeight="21380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1289">
   <si>
     <t>Key</t>
   </si>
@@ -3712,9 +3712,6 @@
     <t>Only two measurements of each test</t>
   </si>
   <si>
-    <t>Figure out with Holger</t>
-  </si>
-  <si>
     <t>Only one repeatability / Handling stress behaviour?</t>
   </si>
   <si>
@@ -3724,9 +3721,6 @@
     <t>Only one repeatability reported although useful data collected</t>
   </si>
   <si>
-    <t>Data is there, needs to be analyses</t>
-  </si>
-  <si>
     <t>Greggor, Alison L.; Jolles, Jolle W.; Thornton, Alex; Clayton, Nicola S.</t>
   </si>
   <si>
@@ -3890,6 +3884,9 @@
   </si>
   <si>
     <t>Probably not useful, but discuss with Holger</t>
+  </si>
+  <si>
+    <t>Discuss with Holger, Data is there but without time between observations, only the mean is meantioned in manuscript</t>
   </si>
 </sst>
 </file>
@@ -4365,9 +4362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE59" sqref="AE59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4640,7 +4637,7 @@
         <v>178</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="7" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4717,7 +4714,7 @@
         <v>190</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4775,7 +4772,7 @@
         <v>86</v>
       </c>
       <c r="AB9" s="8" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4975,7 +4972,7 @@
         <v>57</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5004,7 +5001,7 @@
         <v>8</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="18" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -5033,7 +5030,7 @@
         <v>182</v>
       </c>
       <c r="AB18" s="14" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="19" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5062,7 +5059,7 @@
         <v>150</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="20" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5120,7 +5117,7 @@
         <v>279</v>
       </c>
       <c r="AB21" s="4" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="22" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6056,7 +6053,7 @@
         <v>85</v>
       </c>
       <c r="AB54" s="3" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="55" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -6085,7 +6082,7 @@
         <v>167</v>
       </c>
       <c r="AB55" s="3" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="56" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6140,7 +6137,7 @@
         <v>282</v>
       </c>
       <c r="AB57" s="12" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="58" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -6195,7 +6192,7 @@
         <v>25</v>
       </c>
       <c r="AB59" s="12" t="s">
-        <v>1230</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="60" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -6224,7 +6221,7 @@
         <v>115</v>
       </c>
       <c r="AB60" s="13" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="61" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6282,7 +6279,7 @@
         <v>69</v>
       </c>
       <c r="AB62" s="7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="63" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6311,7 +6308,7 @@
         <v>152</v>
       </c>
       <c r="AB63" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="64" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6398,30 +6395,30 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="11">
         <v>2017</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="J67" s="4">
+      <c r="J67" s="11">
         <v>12</v>
       </c>
-      <c r="AB67" s="4" t="s">
-        <v>1234</v>
+      <c r="AB67" s="11" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="68" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6447,7 +6444,7 @@
         <v>4</v>
       </c>
       <c r="AB68" s="2" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="69" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6478,7 +6475,7 @@
     </row>
     <row r="70" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>396</v>
@@ -6528,7 +6525,7 @@
         <v>24</v>
       </c>
       <c r="AB71" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="72" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6589,7 +6586,7 @@
         <v>153</v>
       </c>
       <c r="AB73" s="2" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="74" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6699,7 +6696,7 @@
         <v>26</v>
       </c>
       <c r="AB77" s="11" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="78" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -6728,7 +6725,7 @@
         <v>66</v>
       </c>
       <c r="AB78" s="13" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="79" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6757,7 +6754,7 @@
         <v>79</v>
       </c>
       <c r="AB79" s="2" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="80" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6861,7 +6858,7 @@
         <v>35</v>
       </c>
       <c r="AB83" s="2" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="84" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6887,7 +6884,7 @@
         <v>9</v>
       </c>
       <c r="AB84" s="2" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="85" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6939,7 +6936,7 @@
         <v>284</v>
       </c>
       <c r="AB86" s="4" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="87" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6968,7 +6965,7 @@
         <v>329</v>
       </c>
       <c r="AB87" s="2" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="88" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -6994,7 +6991,7 @@
         <v>57</v>
       </c>
       <c r="AB88" s="14" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="89" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7020,7 +7017,7 @@
         <v>12</v>
       </c>
       <c r="AB89" s="2" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="90" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7124,7 +7121,7 @@
         <v>81</v>
       </c>
       <c r="AB93" s="2" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="94" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7292,7 +7289,7 @@
         <v>284</v>
       </c>
       <c r="AB99" s="4" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="100" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7321,7 +7318,7 @@
         <v>114</v>
       </c>
       <c r="AB100" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="101" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7408,7 +7405,7 @@
         <v>84</v>
       </c>
       <c r="AB103" s="2" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="104" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7466,7 +7463,7 @@
         <v>68</v>
       </c>
       <c r="AB105" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="106" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7527,7 +7524,7 @@
         <v>165</v>
       </c>
       <c r="AB107" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="108" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7556,7 +7553,7 @@
         <v>68</v>
       </c>
       <c r="AB108" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="109" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7611,7 +7608,7 @@
         <v>2</v>
       </c>
       <c r="AB110" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="111" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7724,7 +7721,7 @@
         <v>220</v>
       </c>
       <c r="AB114" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="115" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7779,7 +7776,7 @@
         <v>91</v>
       </c>
       <c r="AB116" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="117" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7834,7 +7831,7 @@
         <v>133</v>
       </c>
       <c r="AB118" s="2" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="119" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8034,7 +8031,7 @@
         <v>19</v>
       </c>
       <c r="AB125" s="17" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="126" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8205,7 +8202,7 @@
         <v>47</v>
       </c>
       <c r="AB131" s="15" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="132" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -8234,7 +8231,7 @@
         <v>80</v>
       </c>
       <c r="AB132" s="15" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="133" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8321,7 +8318,7 @@
         <v>52</v>
       </c>
       <c r="AB135" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="136" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8350,7 +8347,7 @@
         <v>27</v>
       </c>
       <c r="AB136" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="137" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8379,7 +8376,7 @@
         <v>70</v>
       </c>
       <c r="AB137" s="2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="138" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8410,7 +8407,7 @@
     </row>
     <row r="139" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B139" s="7" t="s">
         <v>761</v>
@@ -8466,7 +8463,7 @@
         <v>26</v>
       </c>
       <c r="AB140" s="2" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="141" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8495,7 +8492,7 @@
         <v>119</v>
       </c>
       <c r="AB141" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="142" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8524,7 +8521,7 @@
         <v>124</v>
       </c>
       <c r="AB142" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="143" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8582,7 +8579,7 @@
         <v>585</v>
       </c>
       <c r="AB144" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="145" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8611,7 +8608,7 @@
         <v>123</v>
       </c>
       <c r="AB145" s="2" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="146" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8672,7 +8669,7 @@
         <v>85</v>
       </c>
       <c r="AB147" s="2" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="148" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8701,7 +8698,7 @@
         <v>3</v>
       </c>
       <c r="AB148" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="149" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8730,7 +8727,7 @@
         <v>123</v>
       </c>
       <c r="AB149" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="150" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8759,7 +8756,7 @@
         <v>46</v>
       </c>
       <c r="AB150" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="151" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8788,7 +8785,7 @@
         <v>133</v>
       </c>
       <c r="AB151" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="152" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8843,7 +8840,7 @@
         <v>126</v>
       </c>
       <c r="AB153" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="154" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8898,7 +8895,7 @@
         <v>5</v>
       </c>
       <c r="AB155" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="156" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8930,7 +8927,7 @@
         <v>69</v>
       </c>
       <c r="AB156" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="157" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8982,7 +8979,7 @@
         <v>872</v>
       </c>
       <c r="AB158" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="159" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9011,7 +9008,7 @@
         <v>122</v>
       </c>
       <c r="AB159" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="160" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -9037,7 +9034,7 @@
         <v>4</v>
       </c>
       <c r="AB160" s="4" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="161" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9092,7 +9089,7 @@
         <v>89</v>
       </c>
       <c r="AB162" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="163" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9118,7 +9115,7 @@
         <v>898</v>
       </c>
       <c r="AB163" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="164" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -9150,7 +9147,7 @@
         <v>28</v>
       </c>
       <c r="AB164" s="4" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="165" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -9176,7 +9173,7 @@
         <v>72</v>
       </c>
       <c r="AB165" s="14" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="166" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9205,7 +9202,7 @@
         <v>18</v>
       </c>
       <c r="AB166" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="167" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9234,7 +9231,7 @@
         <v>75</v>
       </c>
       <c r="AB167" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="168" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9265,7 +9262,7 @@
     </row>
     <row r="169" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>926</v>
@@ -9289,7 +9286,7 @@
         <v>107</v>
       </c>
       <c r="AB169" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="170" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9321,7 +9318,7 @@
         <v>165</v>
       </c>
       <c r="AB170" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="171" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9350,7 +9347,7 @@
         <v>99</v>
       </c>
       <c r="AB171" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="172" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -9379,7 +9376,7 @@
         <v>22</v>
       </c>
       <c r="AB172" s="17" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="173" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9431,7 +9428,7 @@
         <v>109</v>
       </c>
       <c r="AB174" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="175" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9489,7 +9486,7 @@
         <v>124</v>
       </c>
       <c r="AB176" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="177" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9515,7 +9512,7 @@
         <v>10</v>
       </c>
       <c r="AB177" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="178" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9593,7 +9590,7 @@
         <v>27</v>
       </c>
       <c r="AB180" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="181" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -9619,7 +9616,7 @@
         <v>7</v>
       </c>
       <c r="AB181" s="16" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="182" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -9648,7 +9645,7 @@
         <v>80</v>
       </c>
       <c r="AB182" s="11" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="183" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9677,7 +9674,7 @@
         <v>123</v>
       </c>
       <c r="AB183" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="184" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9706,7 +9703,7 @@
         <v>106</v>
       </c>
       <c r="AB184" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="185" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9735,7 +9732,7 @@
         <v>89</v>
       </c>
       <c r="AB185" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="186" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9790,7 +9787,7 @@
         <v>84</v>
       </c>
       <c r="AB187" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="188" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9845,7 +9842,7 @@
         <v>68</v>
       </c>
       <c r="AB189" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="190" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9874,7 +9871,7 @@
         <v>119</v>
       </c>
       <c r="AB190" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="191" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9903,7 +9900,7 @@
         <v>153</v>
       </c>
       <c r="AB191" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="192" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9932,7 +9929,7 @@
         <v>117</v>
       </c>
       <c r="AB192" s="2" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="193" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9961,7 +9958,7 @@
         <v>89</v>
       </c>
       <c r="AB193" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="194" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10013,7 +10010,7 @@
         <v>64</v>
       </c>
       <c r="AB195" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="196" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -10042,7 +10039,7 @@
         <v>113</v>
       </c>
       <c r="AB196" s="17" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="197" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10071,7 +10068,7 @@
         <v>91</v>
       </c>
       <c r="AB197" s="2" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="198" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10100,7 +10097,7 @@
         <v>124</v>
       </c>
       <c r="AB198" s="2" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="199" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10178,7 +10175,7 @@
         <v>21</v>
       </c>
       <c r="AB201" s="2" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="202" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -10210,7 +10207,7 @@
         <v>4</v>
       </c>
       <c r="AB202" s="4" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="203" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10265,7 +10262,7 @@
         <v>145</v>
       </c>
       <c r="AB204" s="14" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="205" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10294,7 +10291,7 @@
         <v>42</v>
       </c>
       <c r="AB205" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="206" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10346,7 +10343,7 @@
         <v>183</v>
       </c>
       <c r="AB207" s="7" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="208" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10375,7 +10372,7 @@
         <v>305</v>
       </c>
       <c r="AB208" s="2" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="209" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10404,7 +10401,7 @@
         <v>133</v>
       </c>
       <c r="AB209" s="2" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="210" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10433,7 +10430,7 @@
         <v>20</v>
       </c>
       <c r="AB210" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="211" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10488,7 +10485,7 @@
         <v>124</v>
       </c>
       <c r="AB212" s="2" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="213" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10517,7 +10514,7 @@
         <v>80</v>
       </c>
       <c r="AB213" s="2" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="214" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10569,7 +10566,7 @@
         <v>169</v>
       </c>
       <c r="AB215" s="2" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="216" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10676,12 +10673,12 @@
         <v>208</v>
       </c>
       <c r="AB219" s="2" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>